<commit_message>
Merge finish with indeed, linkedin, zipRe
</commit_message>
<xml_diff>
--- a/Job Hunter/exceltestsheet/LinkedInJobs.xlsx
+++ b/Job Hunter/exceltestsheet/LinkedInJobs.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <x:si>
     <x:t>Job Title</x:t>
   </x:si>
@@ -55,11 +55,96 @@
     <x:t>URL</x:t>
   </x:si>
   <x:si>
-    <x:t>Sr Accountant</x:t>
+    <x:t>Senior Revenue Accountant - 100% U.S. remote - must have ASC 606 experience</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-            New York City Metropolitan Area
+            New York, NY
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+                Full-time · Associate
+              </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+          Sprinklr is a unified customer experience management (Unified-CXM) platform for modern enterprises with employees around the world helping ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2779839706/?eBP=CwEAAAF9Bj6K4tLLKJhFCkKTrryn3lkPn3AeyH1-u7gosBYPQyE-yeivi5k53x5v9zcWXjFbSSujuNSgP1A_M_aRyx_5sB-dpoD81-nZqQKe36HFB7KNmvKzzIx-oMDNll-FO4m3xmqsSGmu5gEppr4bzA1IlpQ6AcreDZUzLLjLv9qBUtKXCuhdzemJVJj1AZqb0IDzC7Ko3_SjVm0qdoe9EhITUQdQlFiQSei7QIjB7zs46uXPMwhd9VrrOyIKrknuKpGwvT4avHRhYgyrZm2EUlYI2mA2WfGEMtmztNhIWrEV92kfrLk0YBq3X5u1LKgimf2B9-Ru2ueF638wzDnV8_Q&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=N2utwGwQy7URjRXr%2BwTW5w%3D%3D&amp;trackingId=U%2FsZwMQrr8v%2BrDP0YX8KAg%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Junior Tax Accountant</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            Frisco, TX
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            White Plains, NY
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+          Overview
+ Join an award-winning company! 
+ Who are we? 
+Since 1967, Toll Brothers has been building luxury homes and communities in the ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2749242015/?eBP=CwEAAAF9Bj1r8yOxaezlYU-hx1pRXAKXGQNqxLp6UrgEV42_wwj7isrnduXAiV6Nzy7jup40JQGOTiVsJ-O0zh7beFxBvBeqJ8960DgYH5oVmXgDUMpXCWGXuycDbZeE_Z6h7LBH52hqRlih-brLhnhx0BA7gLjaXEPmQCFyMjqNrRxE98SL-EcJ7y2C-W8hyp4ilMgPO0_oonU59M9uN_DWhZ5vs8isjSU9x7nJKyJU4lmmAXuzZddetu9dRn63H3BFyBHc0W6-5bEAw3IvmHkpwUyIkhK8UPhaimtXQRaWkeHt0zH2PRx23QAwPOJhNhrlEuLMMsL_Bn21_aJt-Nw0I0YzmWgLdcqCpqPBdVfnREtU3olZBaQYhYKx_FKw&amp;recommendedFlavor=COMPANY_RECRUIT&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=mw29mCm4ze0iELgn8bIn9g%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Volunteer: Build Site Volunteers Needed!</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            Garland, TX
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+                Volunteer · Associate
+              </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+          Habitat for Humanity of Greater Garland, an ecumenical housing ministry, builds communities of hope, dignity and self-worth through the con...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2786581996/?eBP=CwEAAAF9Bj1r83MWGY_JCSuxA0gbnzUFlI_6pAHNHzwy3rvWt_R_DWMKEb30DGzWLZFMYwm7J_8At1vFgBbJIDa72MVv4c9ce4TUnDGX6d3JLrIR-oRa_PRri-RNoc0HckMRLXug73RQNsC6xNm9jFvd1sCC5mbwjLZafnyK5hZ16wN4gUMBhr-dUZHfVnH2PoHSC-jVm3Qb3J9dSltX3sQk1P7LaFtImSKJMrsNFDceZAf31koijigcWct6ImtTNhd6zoL4d0gO_kNdtaljMPQYKyg0k0mLSo3tuUsf-yzxY3Y1WkHjspl-z0SpsoaQMQ0qcISZaq0j2AN4MLLXmTRMNuGn3czl__TjhkPywZqNT_9U66mf-l1S6FaKTA&amp;recommendedFlavor=JOB_SEEKER_QUALIFIED&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=AGQ72sVDeCCDy97%2Fa%2BYA5Q%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Construction Manager</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            Grand Prairie, TX
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+                Full-time · Mid-Senior level
+              </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+          Texas Home Builder seeking Construction Managers
+This Jobot Job is hosted by Henry Chan
+Are you a fit? Easy Apply now by clicking the "Ap...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2775979794/?eBP=CwEAAAF9Bj1r873G28ycvxvikLQsB_QVfk-BSuwR4BMpBKmOnfOS7MHJ6ghpl88KeSJnzw-V4taJMD2ujwZ3VwF487Z9nil92I3_XzghHSTro73qwC_n2ana2Bi-2WHU5-cAI67fpGMf4-7x10cD-7svkzjvj5kCHRjE5RjoIivqJvSoaqBgNydAa_KS73nMVGsfQqAp9epKp0Vm3MVtZY9BXVgkURlbVjXo80ede9oNHWCZb1saEz-Yku0LCaSoTUKWvAJn_KgBSxfi7q10anvEppBTVWdRR662b1AIIF9uvoV0731wZSvebTeSN_TOhpe3fMzYfqNKw_dE4QT8xgebQ8fIFQp4DiPDD5zLoGu6acab1w8YN2QS-VDGl_FP&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=QDOABJQbJEGYO5Zs7bSvRg%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Member Care Assistant</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            Dallas, TX
           </x:t>
   </x:si>
   <x:si>
@@ -69,134 +154,81 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-          Before applying to this job, please make sure it's the most ideal fit for you! Review our departments and how different jobs compare to one...</x:t>
+          The perfect candidate will provide exceptional customer service with a smile so big you can hear it through the phone. The perfect candidat...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2783593747/?eBP=CwEAAAF9A0_a2A8gRDvfJli08UR4mBpjzvxBcYYSaQWzT6F7f_DSDzXc_WwFox5QAbTK0_7HOQeGEFsMJhqhw8B6PCONkcLLUD_aOg4tCU8ahyq6WSSLDntnK6GhUQQgyZoftCTKW6mOMS0iJt_jpB8LWrX8ij6MLn_0FNv3l881uVXQwiFkEUEZbBNEgZ44V1n5MTj889ZiM491fF2w-PDR4v7rxcDG60VlJ7myDGu8m6BawGZ8xZj0zj8IxwfYyjdDA6Np0vrMag1ID7Xo_vwZQ2UHOMtK2Wi88R7LA99KrI1BOVd6ZXPFKPEFi0KTC9SkAmvaEFMCsMMgDCCcTPrdjQfBlCtr8qtPvXhx0qvJUo9McOR4nnBCyiO_xA&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=QnBDEQPh8FqwWNivDALVtQ%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+    <x:t>https://www.linkedin.com/jobs/view/2790554339/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=JOB_SEEKER_QUALIFIED&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=MfFGd8zbR%2FwJ8RO0qvLUKQ%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
   </x:si>
   <x:si>
-    <x:t>Tax Accountant</x:t>
+    <x:t>RESTAURANT / HOSPITALITY EXPERIENCE - Entry Level Positions</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-            Scarsdale, NY
+            Dallas-Fort Worth Metroplex
           </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                $52,000/yr - $81,000/yr (LinkedIn est.) · Full-time
+                Full-time · Entry level
               </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-          This position is for a full-time tax preparer responsible for tax preparation for individuals and small businesses. The position requires t...</x:t>
+          Are you seeking an opportunity where you can drop anchor and build a career? Our promotional marketing firm has immediate positions availab...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2787317348/?eBP=CwEAAAF9A0_a2EEW6TKx9TbzTYNpgwF-srGT4_YJIz-hDnuuhWWlSrbXeJR0lViw-zqsoOlp6_VvZRRzH1lyhFrYQPEFUsES4x918ObY4VljTQGB2y_85fdXLY5NmI8MZtIQCJbqluxe4nNyKlpVCgu5KErvDMW7GSS0Zdk0KnCOkMWflvka1WyrP_rDtfMPE1rZc5WXyfxLIVt0Jrz7qSm-pHF3nbLOZiCUkAVdMxLfSdNIUBwGFiH6jHFa3G8isB11oXpqAlBYg270j9WUtPOoPx08tgWw-_uv-qoSvjNhpzQfRUW3ipLQhMyzCd1b8ocfTN8SR2tQlO9VrkBzjds8wYqSIAKQ0qemtpa_WczTKqOgdZv9Ds19bA5-oQ&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=vCW%2F6kqLjia3xrfzAn6dDw%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+    <x:t>https://www.linkedin.com/jobs/view/2791924958/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=UZgHnXaGLFi4JtGVc1kluA%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
   </x:si>
   <x:si>
-    <x:t>Accountant</x:t>
+    <x:t>Local Construction Superintendent - Tilt Wall projects</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-            New York, NY
+          Local Superintendent, ENR Ranked Design Build Industrial General Contractor
+This Jobot Job is hosted by Eli Mandelbaum
+Are you a fit? Eas...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2778658271/?eBP=CwEAAAF9Bj1r8xBHob3KywHaU0keF5f3pQyfRrZeEOKzLRcICactERbEkvXpUqrqNZp6pX-q-S1FPJKM4ZCuy603XGkIZ16z4U4s4gYk9b_6mnD1_oYp4GIPaYPrJlcZSIGvt2ZWuv4jHt_fdT9ucPhJjI6HC1nlU9XuqEVnZpxlnLptoNWtszY6QsihvUPUy2KAuxYSj8wZMCD2IyGgAtUqR3qmuyQC7QgYvR1fGGd8ju_wYOMRAgKUzeeumhSQBlXaDF0g02NSlh9N8w1y3WoRdXY9rWR3f_926tQAxuOMG17Mj6TCweHHkwJbeg-fJbBozeUHn4Su1JTU6r-VXi7F3HF4q079gdMztiSC3sCEtlgdZhklsXSwh57wJy2J&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=IwXNzMZfNS9UmaJwWGI%2Fkw%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Construction Superintendent - Multifamily</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+          This Jobot Job is hosted by Jordon Cox
+Are you a fit? Easy Apply now by clicking the "Apply" button and sending us your resume.
+A Bit Abo...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2779402183/?eBP=CwEAAAF9Bj1r88mNgc8Bj4izdr1uWfrytf2mOyQlXM_AX6xR4diuyIk6NVnX2NHsLeDAUORZF8SQ4ubVlva_pnXHislKxZtQFCE4nyDA73am_OxA3q3jgdh-PdagXbC3ixmS4AL7cqg2EY8IZdGiW12hu_l3ZpfdPsYrL_HMKNA-SUzHf2Ejud33cKtCN71bUeEb5dTwim178G_Gg-pElyrboWWyKfpzpCUHQtZRVfAeSGAXS2ZELc3kA1xzWPWZSeJ2hCkvZZ-eBW8RiIO84HzfjFvPhEGNBgiv4nH8uwvVR2t1VqOuf7UNG7PqXkufvmeFUWhjnEoqzS-VQ-lsO1asNOpj3f89n5SZiZ1IsmCSFRPgGgf2tZ8BFHJvsrg-&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=iNJiB%2F6G1HJUgTI4%2F8YGLw%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            McKinney, TX
+          </x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/jobs/view/2775978793/?eBP=CwEAAAF9Bj1r8zkA1xActwusKpIr3rKftcQi2-a-kRR__fKLsKStTcyjF9_VkfypBS90PJhH44BnAagqq2p1qUYrEDJS5-JLe_kG7rvLCk0Y1i5UrQ9B7N_7Et33T0pG690KxDKybJlkQRVVHh3XcXMMJGiNpMKrgs9Ndvq6FZKcTdI4FaItmdmoFh2upLjspCl1Iwk_84euUVGAUYjOQomPbKJ9nHmWZ0oalwsV4ce4Np7NG2Ml_I6PltEvPxU4biE9Zkd8aJWbOvW1gNnNKdafb2yJC3tuDTaSVFaQ7ZCzqrIPQiNtSJbSqGkbLHirykFr3tPhJOxqvvuq5PRWA72mGTKF76TyJYz8cDWh8fACxNbWtp8W44_GusY8puYE&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=uEeq%2FBf34sE4hpDw7O0aEw%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Roofing Sales Rep, New Construction</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+            Irving, TX
           </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                Contract
-              </x:t>
+          Location: DFW
+Pay: base 55-65k + commission
+Direct hire
+The Role
+We have an immediate need for a roofing sales rep with new constructio...</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">
-          (part-time; average 8 hours/week; seeking candidate who specializes in non-profits)
-The Citizens Budget Commission (CBC), New York’s leadin...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2785218550/?eBP=CwEAAAF9A0_a2D5YFRve1WlGPeIIqjQ9E1jmfh4Q7rutwU6od0Lb7DIw6Sg2lSfW9QS9v372ImfDi4UKXw4YMm4Yw9s4B8THQ1pyRcpkIt8vZMTMu7GTjFdkCb37X9yh404BQDlBziQ4IeeGx4lAR2oyDThaPUyqgeRBgMI0oaSYHRFV0ysrSYg-xRIOFYSeDFDq7_sD1Ko5QuktXgtonZ4jz9QdbcCbSHkwCZit-gyrWWNH8Arg6l7SnxbRrtRGx5_leaJlqYoV_4zXI5RGGvbfz4TMk1OIF0T2HNd_JcDKm-9CpS4Nc6TXuSmA8A8pqlXIh_wrEP2z_-bbKbnOfWN--OHIggooZgUMZfMdnPlev2gtst7EugdrR-w7Ofjo&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=KXcz62jYCWgVd%2BqUGMq9vA%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Entry-Level Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-            Manhattan, NY
-          </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-                Full-time · Associate
-              </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          Our client is a digital marketing firm is hiring for their Entry-Level Accountant Positions. The company has a great work hard play hard me...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2780696661/?eBP=CwEAAAF9A0_a2Kg6-Mzw0FeJmuuXnn2yHq87UDQE9HZCifv2TXW4j4bM8Lmqlr8MeUTpIdoMi9aEQdoUTDLk6A6_RO_V-Vr8jGu3JXjqRFj0BqbsXCfnEazVED7Bk2vieo9ZS33BCXSYLETQFBDDwTHh4vTCNOHyjsCmQxsaYWy3P6AeLdyXBPEfOPDQUlcp6GBeDzEc6hdJISU_0CgUjNnWmbwNNtndbwE424P3aQmCZ_-FMLZc-S4dYo0t0ThFjRPqVZOH0bV5mzlR3A5j8f6EOhCQTeCp0HSNKk8KqC0TuprPKR49ZyTeu3yYkzdyJOI7TB04Rg0uePo0miaMQERu3wjbbXpP1IxvJ2HW36lN3jqs9La97iJi_L3nHpiJ&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=PtxoFn6nvl6bMJ%2Fmw2180w%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          SIMULATE's mission is to accelerate the world's transition to sustainable nutrition. Our first product, NUGGS, is a chicken nugget simulati...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2786815214/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=5UkQ1qhkDibwELu5gG19Bg%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-            Stamford, CT
-          </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          Summary
- Accountant Job Description 
-WWE seeks a motivated, experienced Accountant to join our General Accounting team. The ideal candida...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2786681352/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=AUju8bHJrfP0%2FzaoLglRcQ%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sr. Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          Description
-Are you a quick learner who can keep up in a fast-paced environment? Are you excited about the chance to be part of a renowned...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2784073893/?eBP=CwEAAAF9A0_a2JfJ2Ulbl5a--t0H-n72Qj0I1-_4Yk_KFPnR1ILw6suiiq-IOa5Z9lBjZoj-29IoQkdbTKp3voWSn7BJXTWSbQ8cP95i8KhGF1RqMBufxBgYC0HRK4t6BmrwwLknuBRN7fNw_ZOKiQ4dF_9AkbqSpafWM8tOMshmc6SOiBqS1Iq84RhNLwvM4QsvN8WbvNv64Q2tf-AvNcheVbk1prlCkSo_W_6s5b7UO9tIbI8AQXhUZiam3vk4eTP_WKvwGZG5aaQQ1xXuBC6zVnJjXHl2Z7cONPLhSk0gvTxCjeIJ77iHsXuKVj2k3JCmXSXM4m2t9GkTWowjBJ_Vi5M4YT6h6Og-6MTAYcKB7L7UgsmjZfNpFirkgYeg&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=To3w2RwOyW34g02PMiVpjA%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Junior Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-           Zeel is looking for a Junior Accountant - a high-energy individual with exceptional organizational skills to join the Finance team at this...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2790511292/?eBP=CwEAAAF9A0_a2CEMlOHgHiqByAbBY8JYlbk423a4cE0ZvLaxibT42mP-ulyAr1jmqeJgZl-I6VhDhdWo7VVGqRy1p5ryMXghpH3mUTr78B0edQm_wrTLMYwQTb0VSS2dg2RJ7MAPVGKCvrnNuAbuupE-9SnxzMp4ei5btDTFuodWWzupSEHgpuPXcfVhbB-h-biL-MXWMQdEtTh4QwF296j3nOuJPHhe8_gTlR1oSj63AEpAoqmwS9lnCJrdo7GjOclWC-xiXfeVAHVUBV6-h6Wgx4OmzSs1X-uvwJ-o9tQwuP4JKpyNlsPe284IgUc2XMQxHGMPqsRJrIqMyYNDvkGefUT9UBlEIuqhKuImRGArelyk7wpEpI4mHoer3BkX&amp;recommendedFlavor=JOB_SEEKER_QUALIFIED&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=1YM4n2%2BzRRjAel1lS5QHYA%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Revenue Accountant - 100% U.S. remote - must have ASC 606 experience</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          Sprinklr is a unified customer experience management (Unified-CXM) platform for modern enterprises with employees around the world helping ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2779840708/?eBP=CwEAAAF9A0_a2Xzrm_H6Xwsz_oO-abPSg_ZeQE4c5yu1lKOgZD82-mzBkcog3kRDY9-pvUndevExZBCYWzN6_9sD49LVRZ98ak_CGsMTAYymgd1NzUF1cqdiNwmy5r1_E1L-p8rr52DnfknRwdNhVk0X4yVpsCaBiyjjpTRF6gFBQltPV-UeDZSPW8sWtJQK79vpvMyNcN-XfbLK1H_xdk60PXU2Qc0f-mH7-DQUcQUz7n1JlfOosTboEbHDzs6_oM5GfCR-ZEG_itVxJr1PQkRGxriGltmyhK4-Rotn5gcYsivkMECzGQ3qkj6ocAqUODIqQAL4cR2_b4RWBT7N9KTyXbR0Bk2zqAhD5knLQg7ixNSSs8Bmz5W1W5SD4u55&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=FbcKf%2FJaAEAv0B15uCpjDw%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Label Services Group Senior Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-          Who we are: 
-Take-Two develops and publishes some of the world's biggest games. Our Rockstar label creates Grand Theft Auto and Red Dead R...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.linkedin.com/jobs/view/2722221448/?eBP=CwEAAAF9A0_a2al4YKDrTkw-GJKNtikPxIBFjgwtC_yN3v4wfYDlm773oiaxBCs1-gJwg0NtK53h5rkK-0RYzg176mo-kj4ndkaTVsr_JGynNLgkt0vtdT5bhkFTpT1e2-yVMNK8093hWTv8wuHMts1tz03OxTpRH__P_QxwSmdhx5VofhoQjxFcPusgFozfCLmyF8V2-RtFmOh0MCG4R8IS4fssUHChr4ob6dlTm5NS_9F7X6EO3544goDObJEejz-BLb1aQwvi3h7Pn6FCqUd9gW0y3kXoDDdY7ms5UHgvIcRssLYUDqB6U6LqkWbaG63KJhJQqbXh1r0_a2o0GROwJv2UACy03aqOWB-g_3GiRIlQGdXOjPQLT85XEnxK&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=yD3FIZOV9coyLD4pa9AJlQ%3D%3D&amp;trackingId=f%2B50u6IvO%2BX7RWuJEsK7BQ%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
+    <x:t>https://www.linkedin.com/jobs/view/2783010603/?eBP=CwEAAAF9Bj1r9IxAg0znB6f7i22O5DSvNfiy7PkeZCUIco4nE4Z0nfINYgsI4cWj2DxMtrd-B9r2YB_vnTVDVnHboTLffCTTcuRrkOQGa5meOy1jLb6mZl3YaGqkuCHQjtdpei9-nfArxymc6ioWHljU_zQfSWOXJ8mrbxTMDYn5r7zbRJyZzL3BF3EHhNFocrlZgnK_zRMEBJBALuvjg-FIvdxOirYZumzae18Nc0Mr4j2lfKdvqTp4E1XtbueoFgcPJqL4cSafy_29rQu7Mno6EcBkIPewektXvwYxxBD-g57S4j-3kQgD5Np7aRwj-IxNJnEPRvTEQghFJNbmHYxir7MM2hnWax_-9x9jVl6-J1Di3259YIma2QbfX8-S&amp;recommendedFlavor=COMPANY_RECRUIT&amp;refId=XQWPTMUwS%2BAokBD3FAcHeA%3D%3D&amp;trackingId=5tTq%2FtP%2FNZhiCFa4zfvC4A%3D%3D&amp;trk=flagship3_search_srp_jobs</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -239,8 +271,1028 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3662">
+  <x:cellStyleXfs count="4002">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -11647,10 +12699,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C3" s="7" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>13</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E3" s="12" t="s">
         <x:v>14</x:v>
@@ -11701,122 +12753,122 @@
     </x:row>
     <x:row r="6" spans="1:6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A6" s="7" t="s">
-        <x:v>16</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B6" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C6" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D6" s="7" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E6" s="8" t="s">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F6" s="7" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" customFormat="1" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A7" s="7" t="s">
-        <x:v>16</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B7" s="7" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C7" s="7" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D7" s="7" t="s">
-        <x:v>23</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E7" s="8" t="s">
-        <x:v>29</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F7" s="7" t="s">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="7" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B8" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C8" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D8" s="7" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="E8" s="8" t="s">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F8" s="7" t="s">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="7" t="s">
-        <x:v>34</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B9" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C9" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D9" s="7" t="s">
-        <x:v>8</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E9" s="8" t="s">
-        <x:v>35</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F9" s="7" t="s">
-        <x:v>36</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6" customFormat="1" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B10" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C10" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D10" s="7" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="E10" s="8" t="s">
-        <x:v>38</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F10" s="7" t="s">
-        <x:v>39</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="7" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B11" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C11" s="7" t="s">
-        <x:v>17</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D11" s="7" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="E11" s="8" t="s">
-        <x:v>41</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F11" s="7" t="s">
-        <x:v>42</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>